<commit_message>
Fichier météo updated : 29/06/2011 -> 15%
</commit_message>
<xml_diff>
--- a/ projet-ia/ressource/Projet_Météo.xlsx
+++ b/ projet-ia/ressource/Projet_Météo.xlsx
@@ -1888,21 +1888,22 @@
   <dimension ref="A1:N1476"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G1119" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G154" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G1125" sqref="G1125"/>
+      <selection pane="bottomRight" activeCell="G170" sqref="G170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="18" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" style="18" customWidth="1"/>
-    <col min="3" max="4" width="33" style="18" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" style="18" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="33" style="18" customWidth="1"/>
+    <col min="4" max="4" width="33" style="18" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="18" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="18"/>
     <col min="7" max="7" width="26.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.140625" style="18" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" style="18" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="27.28515625" style="18" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32" style="18" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="30.140625" style="22" bestFit="1" customWidth="1"/>

</xml_diff>